<commit_message>
Mips con pruebas de instrucciones
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb1f0ea9a93514c6/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaspa\Documents\win7VM\workspace\ArquitecturaDeComputadoras\TP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="8_{4FFE7CBC-1771-4A95-92AF-5633C48F0E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B24BA8A-55EF-4CC4-8900-A3E316CCAEA2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB903A1-87A6-4561-A1D9-73FD4A8BBB47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{2210718F-9957-4FB8-8964-C98656C5B862}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Intruccion</t>
   </si>
@@ -316,13 +316,16 @@
   </si>
   <si>
     <t>PM x 32</t>
+  </si>
+  <si>
+    <t>NOP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,6 +372,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -649,30 +661,33 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,34 +1030,34 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="63" t="s">
+      <c r="J2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63" t="s">
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="64"/>
+      <c r="R2" s="68"/>
     </row>
     <row r="3" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
+      <c r="D3" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1301,13 +1316,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC330E5-CC5D-4C8C-BAAB-9D9BC99E15B8}">
-  <dimension ref="A3:AC42"/>
+  <dimension ref="A3:AC44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,14 +1438,14 @@
     </row>
     <row r="6" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="J6" t="s">
         <v>69</v>
       </c>
@@ -1452,14 +1467,14 @@
       <c r="P6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q6" s="66" t="s">
+      <c r="Q6" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
       <c r="W6" s="3" t="s">
         <v>2</v>
       </c>
@@ -3243,7 +3258,7 @@
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="73" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="41">
@@ -3326,7 +3341,7 @@
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="73" t="s">
         <v>48</v>
       </c>
       <c r="C30" s="41">
@@ -3990,7 +4005,7 @@
       </c>
     </row>
     <row r="38" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="73" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="38">
@@ -4320,6 +4335,89 @@
       </c>
       <c r="AC42" s="62">
         <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B44" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="J44" s="56">
+        <v>0</v>
+      </c>
+      <c r="K44" s="56">
+        <v>0</v>
+      </c>
+      <c r="L44" s="56">
+        <v>0</v>
+      </c>
+      <c r="M44" s="56">
+        <v>0</v>
+      </c>
+      <c r="N44" s="56">
+        <v>0</v>
+      </c>
+      <c r="O44" s="56">
+        <v>0</v>
+      </c>
+      <c r="P44" s="56">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="56">
+        <v>1</v>
+      </c>
+      <c r="R44" s="56">
+        <v>1</v>
+      </c>
+      <c r="S44" s="56">
+        <v>1</v>
+      </c>
+      <c r="T44" s="56">
+        <v>1</v>
+      </c>
+      <c r="U44" s="56">
+        <v>1</v>
+      </c>
+      <c r="V44" s="56">
+        <v>0</v>
+      </c>
+      <c r="W44" s="56">
+        <v>0</v>
+      </c>
+      <c r="X44" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="56">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="56">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="56">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="56">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4343,7 +4441,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="63" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4367,7 +4465,7 @@
       <c r="B7" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="64"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -4380,19 +4478,19 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71" t="s">
+      <c r="C11" s="65"/>
+      <c r="D11" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71" t="s">
+      <c r="E11" s="65"/>
+      <c r="F11" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71" t="s">
+      <c r="G11" s="65"/>
+      <c r="H11" s="65" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4400,13 +4498,13 @@
       <c r="B12" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="66" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4525,14 +4623,14 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="68" t="s">
+      <c r="K3" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68" t="s">
+      <c r="L3" s="72"/>
+      <c r="M3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="68"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="4" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D4" s="12">

</xml_diff>